<commit_message>
implemented HW1 for NHPA
</commit_message>
<xml_diff>
--- a/Tutorium Zeitaufwand.xlsx
+++ b/Tutorium Zeitaufwand.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Desktop\Tutorium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC95482-40D4-4F86-92E0-CE6D53EFA0D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CD5735-516F-45F0-A34B-D981DC3BE28B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{D8B358A2-AB3C-4847-A59C-4BB297B950BC}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>Datum</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Std.</t>
+  </si>
+  <si>
+    <t>STL</t>
+  </si>
+  <si>
+    <t>Numerical HP Algorithms</t>
   </si>
 </sst>
 </file>
@@ -406,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1770EE45-9D0B-456C-B849-63504BC5A6C1}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,6 +671,71 @@
         <v>2</v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>43370</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>43381</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>43388</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>